<commit_message>
Update report.html to reflect test results and metadata changes
- Modified the output suite data to update test case identifiers and results.
- Added a new string to the output for the addExpenseTest case.
- Updated statistics to indicate a failure in the addExpenseTest case.
- Adjusted baseMillis and generated values to reflect the latest test run.
</commit_message>
<xml_diff>
--- a/ProjectTest65/Excel/AddExpense.xlsx
+++ b/ProjectTest65/Excel/AddExpense.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5760" yWindow="2496" windowWidth="17280" windowHeight="8112" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3324" yWindow="4128" windowWidth="17280" windowHeight="8112" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddExpense" sheetId="1" state="visible" r:id="rId1"/>
@@ -501,7 +501,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.8"/>
@@ -576,7 +576,7 @@
     <row r="2">
       <c r="A2" s="4" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>N</t>
         </is>
       </c>
       <c r="B2" s="4" t="n">
@@ -604,17 +604,21 @@
       <c r="H2" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="I2" s="1" t="n"/>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="B3" s="1" t="n">
@@ -630,7 +634,7 @@
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>เมล็ดผักซี</t>
+          <t>เมล็ดผักชี</t>
         </is>
       </c>
       <c r="F3" s="1" t="n">
@@ -642,12 +646,21 @@
       <c r="H3" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="I3" s="1" t="n"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>not message</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="B4" s="1" t="n">
@@ -663,7 +676,7 @@
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>เมล็ดผักซี</t>
+          <t>เมล็ดผักชี</t>
         </is>
       </c>
       <c r="F4" s="1" t="n">
@@ -674,15 +687,24 @@
       </c>
       <c r="H4" s="1" t="inlineStr">
         <is>
-          <t>บันทึกข้อมูลสำเร็จ</t>
-        </is>
-      </c>
-      <c r="I4" s="1" t="n"/>
+          <t>บันทึกรายจ่ายสำเร็จ</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>not message</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="B5" s="1" t="n">
@@ -712,7 +734,16 @@
           <t>กรุณาเลือกอุปกรณ์</t>
         </is>
       </c>
-      <c r="I5" s="1" t="n"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>not message</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -733,7 +764,7 @@
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>เมล็ดผักซี</t>
+          <t>เมล็ดผักชี</t>
         </is>
       </c>
       <c r="F6" s="1" t="n">
@@ -745,7 +776,16 @@
       <c r="H6" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="I6" s="1" t="n"/>
+      <c r="I6" s="1" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -766,7 +806,7 @@
       </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t>เมล็ดผักซี</t>
+          <t>เมล็ดผักชี</t>
         </is>
       </c>
       <c r="F7" s="3" t="n">
@@ -780,7 +820,16 @@
           <t>NaN</t>
         </is>
       </c>
-      <c r="I7" s="1" t="n"/>
+      <c r="I7" s="1" t="inlineStr">
+        <is>
+          <t>-10</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -801,7 +850,7 @@
       </c>
       <c r="E8" s="1" t="inlineStr">
         <is>
-          <t>เมล็ดผักซี</t>
+          <t>เมล็ดผักชี</t>
         </is>
       </c>
       <c r="F8" s="5" t="inlineStr">
@@ -817,7 +866,16 @@
           <t>NaN</t>
         </is>
       </c>
-      <c r="I8" s="1" t="n"/>
+      <c r="I8" s="1" t="inlineStr">
+        <is>
+          <t>NaN</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -838,7 +896,7 @@
       </c>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>เมล็ดผักซี</t>
+          <t>เมล็ดผักชี</t>
         </is>
       </c>
       <c r="F9" s="2" t="n"/>
@@ -850,7 +908,16 @@
           <t>กรุณากรอกราคา</t>
         </is>
       </c>
-      <c r="I9" s="1" t="n"/>
+      <c r="I9" s="1" t="inlineStr">
+        <is>
+          <t>กรุณากรอกราคา</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -871,7 +938,7 @@
       </c>
       <c r="E10" s="1" t="inlineStr">
         <is>
-          <t>เมล็ดผักซี</t>
+          <t>เมล็ดผักชี</t>
         </is>
       </c>
       <c r="F10" s="1" t="n">
@@ -883,7 +950,16 @@
       <c r="H10" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="I10" s="1" t="n"/>
+      <c r="I10" s="1" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -904,7 +980,7 @@
       </c>
       <c r="E11" s="1" t="inlineStr">
         <is>
-          <t>เมล็ดผักซี</t>
+          <t>เมล็ดผักชี</t>
         </is>
       </c>
       <c r="F11" s="1" t="n">
@@ -918,7 +994,16 @@
           <t>NaN</t>
         </is>
       </c>
-      <c r="I11" s="1" t="n"/>
+      <c r="I11" s="1" t="inlineStr">
+        <is>
+          <t>-50</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -939,7 +1024,7 @@
       </c>
       <c r="E12" s="1" t="inlineStr">
         <is>
-          <t>เมล็ดผักซี</t>
+          <t>เมล็ดผักชี</t>
         </is>
       </c>
       <c r="F12" s="1" t="n">
@@ -955,7 +1040,16 @@
           <t>NaN</t>
         </is>
       </c>
-      <c r="I12" s="1" t="n"/>
+      <c r="I12" s="1" t="inlineStr">
+        <is>
+          <t>NaN</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -976,7 +1070,7 @@
       </c>
       <c r="E13" s="1" t="inlineStr">
         <is>
-          <t>เมล็ดผักซี</t>
+          <t>เมล็ดผักชี</t>
         </is>
       </c>
       <c r="F13" s="1" t="n">
@@ -992,7 +1086,16 @@
           <t>NaN</t>
         </is>
       </c>
-      <c r="I13" s="1" t="n"/>
+      <c r="I13" s="1" t="inlineStr">
+        <is>
+          <t>NaN</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -1013,7 +1116,7 @@
       </c>
       <c r="E14" s="1" t="inlineStr">
         <is>
-          <t>เมล็ดผักซี</t>
+          <t>เมล็ดผักชี</t>
         </is>
       </c>
       <c r="F14" s="1" t="n">
@@ -1025,7 +1128,16 @@
           <t>กรุณากรอกจำนวน</t>
         </is>
       </c>
-      <c r="I14" s="1" t="n"/>
+      <c r="I14" s="1" t="inlineStr">
+        <is>
+          <t>กรุณากรอกจำนวน</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update multiple Excel files with new data and revisions
</commit_message>
<xml_diff>
--- a/ProjectTest65/Excel/AddExpense.xlsx
+++ b/ProjectTest65/Excel/AddExpense.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\MiniProjectTest\ProjectTest65\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D403F0DF-701F-4288-80C7-E8DEFFAECBCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B4470C-5493-43C5-AA6C-C784D62520F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10695" yWindow="3870" windowWidth="16965" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddExpense" sheetId="1" r:id="rId1"/>
@@ -176,7 +176,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,13 +211,34 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -228,37 +249,55 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -266,11 +305,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="40% - Accent2" xfId="3" builtinId="35"/>
@@ -611,491 +645,492 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.69921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.09765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.796875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="5">
         <v>50</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="5">
         <v>1</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="5">
         <v>50</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="5">
         <v>10</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="5">
         <v>1</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="5">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="4">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="5">
         <v>10</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="5">
         <v>1</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="4">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="5">
         <v>10</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="5">
         <v>1</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="5">
         <v>10</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="4">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="5">
         <v>1</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="4">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="6">
         <v>-10</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="5">
         <v>1</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="4">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="5">
         <v>1</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="11" t="s">
+      <c r="H8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="4">
         <v>8</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="1">
+      <c r="D9" s="9"/>
+      <c r="E9" s="5">
         <v>1</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="12" t="s">
+      <c r="H9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="L9" s="12"/>
-      <c r="M9" s="13" t="s">
+      <c r="L9" s="18"/>
+      <c r="M9" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="4">
         <v>9</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="5">
         <v>10</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="5">
         <v>5</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="5">
         <v>50</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="L10" s="14">
+      <c r="H10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="12">
         <f>COUNTIF(H:H,"Pass")</f>
         <v>11</v>
       </c>
-      <c r="M10" s="14" t="str">
+      <c r="M10" s="12" t="str">
         <f>TEXT(L10/13,"0.00%")</f>
         <v>84.62%</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="4">
         <v>10</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="5">
         <v>10</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="6">
         <v>-5</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="L11" s="15">
+      <c r="L11" s="13">
         <f>COUNTIF(H:H,"Fail")</f>
         <v>2</v>
       </c>
-      <c r="M11" s="15" t="str">
+      <c r="M11" s="13" t="str">
         <f>TEXT(L11/13,"0.00%")</f>
         <v>15.38%</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="4">
         <v>11</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="5">
         <v>10</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="H12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="1">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="4">
+        <v>12</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="5">
         <v>10</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H13" t="s">
-        <v>12</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="H13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="4">
         <v>13</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="5">
         <v>10</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="1" t="s">
+      <c r="E14" s="9"/>
+      <c r="F14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K14" s="11" t="s">
+      <c r="H14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K14" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="K15" s="12" t="s">
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="K15" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="L15" s="12"/>
-      <c r="M15" s="13" t="s">
+      <c r="L15" s="18"/>
+      <c r="M15" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="K16" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="L16" s="14">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="K16" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" s="12">
         <f>COUNTIF(I:I,"Pass")</f>
         <v>9</v>
       </c>
-      <c r="M16" s="14" t="str">
+      <c r="M16" s="12" t="str">
         <f>TEXT(L16/13,"0.00%")</f>
         <v>69.23%</v>
       </c>
     </row>
-    <row r="17" spans="11:13" x14ac:dyDescent="0.3">
-      <c r="K17" s="15" t="s">
+    <row r="17" spans="11:13" x14ac:dyDescent="0.4">
+      <c r="K17" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="L17" s="15">
+      <c r="L17" s="13">
         <f>COUNTIF(I:I,"Fail")</f>
         <v>4</v>
       </c>
-      <c r="M17" s="15" t="str">
+      <c r="M17" s="13" t="str">
         <f>TEXT(L17/13,"0.00%")</f>
         <v>30.77%</v>
       </c>

</xml_diff>